<commit_message>
Script 6 Issue fixing
</commit_message>
<xml_diff>
--- a/Resources/6-data.xlsx
+++ b/Resources/6-data.xlsx
@@ -497,7 +497,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,6 +675,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -843,7 +849,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -928,6 +934,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1277,7 +1284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -2915,7 +2922,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="36" t="s">
         <v>101</v>
       </c>
       <c r="C60" t="s">
@@ -2968,6 +2975,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated script and resource
</commit_message>
<xml_diff>
--- a/Resources/6-data.xlsx
+++ b/Resources/6-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="120">
   <si>
     <t>Order type</t>
   </si>
@@ -364,6 +364,18 @@
   </si>
   <si>
     <t>USTPU25</t>
+  </si>
+  <si>
+    <t>3013697310</t>
+  </si>
+  <si>
+    <t>3013697311</t>
+  </si>
+  <si>
+    <t>3013697312</t>
+  </si>
+  <si>
+    <t>3013697315</t>
   </si>
 </sst>
 </file>
@@ -1311,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V65"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,190 +1453,219 @@
       <c r="T2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="V2" s="33"/>
-    </row>
-    <row r="3" spans="1:22" s="34" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
+      <c r="V2" s="33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="33">
+        <v>2</v>
+      </c>
       <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="V3" s="33"/>
-    </row>
-    <row r="4" spans="1:22" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S3" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="V3" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="33" t="s">
         <v>106</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I4" s="33">
-        <v>2</v>
-      </c>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="T4" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="V4" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="33" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="33">
+        <v>1</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="S5" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="33">
+        <v>3013697313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D6" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="33" t="s">
+      <c r="E6" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="33">
+        <v>2</v>
+      </c>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="T6" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="33">
+        <v>3013697314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H7" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="33">
-        <v>1</v>
-      </c>
-      <c r="R5" s="33" t="s">
+      <c r="I7" s="33">
+        <v>1</v>
+      </c>
+      <c r="R7" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="33" t="s">
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="V8" s="33"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" s="33">
-        <v>1</v>
-      </c>
-      <c r="R6" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="S6" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="T6" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" s="33">
-        <v>2</v>
-      </c>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="T7" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="U7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="I8" s="33">
-        <v>1</v>
-      </c>
-      <c r="R8" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="V9" s="33"/>
+      <c r="H9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="7">
+        <v>12</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -1637,12 +1678,12 @@
         <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="31" t="s">
         <v>85</v>
       </c>
       <c r="I10" s="7">
@@ -1654,7 +1695,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>57</v>
@@ -1663,10 +1704,10 @@
         <v>66</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="H11" s="31" t="s">
         <v>85</v>
@@ -1680,25 +1721,25 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>85</v>
+        <v>8</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="I12" s="7">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="U12" s="1">
         <v>1</v>
@@ -1706,7 +1747,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
@@ -1715,12 +1756,12 @@
         <v>65</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="31" t="s">
         <v>87</v>
       </c>
       <c r="I13" s="7">
@@ -1732,25 +1773,25 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I14" s="7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="U14" s="1">
         <v>1</v>
@@ -1770,7 +1811,7 @@
         <v>11</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>85</v>
@@ -1796,7 +1837,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H16" s="31" t="s">
         <v>85</v>
@@ -1816,19 +1857,19 @@
         <v>57</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="7">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="U17" s="1">
         <v>1</v>
@@ -1836,22 +1877,22 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I18" s="7">
         <v>1</v>
@@ -1862,25 +1903,25 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I19" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="U19" s="1">
         <v>1</v>
@@ -1900,7 +1941,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="H20" s="31" t="s">
         <v>85</v>
@@ -1926,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>85</v>
@@ -1952,7 +1993,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="H22" s="31" t="s">
         <v>85</v>
@@ -1978,7 +2019,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="H23" s="31" t="s">
         <v>85</v>
@@ -1992,25 +2033,25 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I24" s="7">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U24" s="1">
         <v>1</v>
@@ -2020,7 +2061,7 @@
       <c r="A25" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -2030,7 +2071,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="H25" s="31" t="s">
         <v>84</v>
@@ -2038,39 +2079,39 @@
       <c r="I25" s="7">
         <v>24</v>
       </c>
-      <c r="U25" s="1">
+      <c r="U25" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>74</v>
+      <c r="A26" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I26" s="7">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="U26" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>75</v>
+      <c r="A27" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>57</v>
@@ -2081,8 +2122,8 @@
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>64</v>
+      <c r="F27" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="H27" s="31" t="s">
         <v>85</v>
@@ -2096,25 +2137,25 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="31" t="s">
-        <v>85</v>
+        <v>37</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="I28" s="7">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="U28" s="34">
         <v>1</v>
@@ -2122,7 +2163,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>57</v>
@@ -2134,13 +2175,13 @@
         <v>11</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H29" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="31" t="s">
         <v>86</v>
       </c>
       <c r="I29" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U29" s="34">
         <v>1</v>
@@ -2148,7 +2189,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>57</v>
@@ -2166,7 +2207,7 @@
         <v>86</v>
       </c>
       <c r="I30" s="7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="U30" s="34">
         <v>1</v>
@@ -2174,7 +2215,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>57</v>
@@ -2183,7 +2224,7 @@
         <v>68</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>63</v>
@@ -2192,15 +2233,15 @@
         <v>86</v>
       </c>
       <c r="I31" s="7">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="U31" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>78</v>
+      <c r="A32" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>57</v>
@@ -2209,10 +2250,10 @@
         <v>68</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="H32" s="31" t="s">
         <v>86</v>
@@ -2244,7 +2285,7 @@
         <v>86</v>
       </c>
       <c r="I33" s="7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="U33" s="34">
         <v>1</v>
@@ -2261,7 +2302,7 @@
         <v>68</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>32</v>
@@ -2270,15 +2311,15 @@
         <v>86</v>
       </c>
       <c r="I34" s="7">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="U34" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>80</v>
+      <c r="A35" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>57</v>
@@ -2287,75 +2328,93 @@
         <v>68</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H35" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="7">
+        <v>1</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35" s="22"/>
+      <c r="U35" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="12">
+        <v>4</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="I35" s="7">
-        <v>10</v>
-      </c>
-      <c r="U35" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="7">
-        <v>1</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36" s="19" t="s">
-        <v>90</v>
-      </c>
       <c r="M36">
         <v>1</v>
       </c>
-      <c r="N36" s="20" t="s">
-        <v>91</v>
+      <c r="N36" s="24" t="s">
+        <v>95</v>
       </c>
       <c r="O36">
         <v>1</v>
       </c>
-      <c r="P36" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-      <c r="R36" s="22"/>
       <c r="U36" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>77</v>
+      <c r="A37" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>57</v>
@@ -2363,87 +2422,69 @@
       <c r="D37" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="11" t="s">
+      <c r="E37" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="H37" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="I37" s="12">
-        <v>4</v>
-      </c>
-      <c r="J37" s="23" t="s">
+      <c r="I37" s="17">
+        <v>5</v>
+      </c>
+      <c r="J37" s="25" t="s">
         <v>93</v>
       </c>
       <c r="K37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L37" s="33" t="s">
         <v>86</v>
       </c>
       <c r="M37">
-        <v>1</v>
-      </c>
-      <c r="N37" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N37" s="27" t="s">
         <v>95</v>
       </c>
       <c r="O37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U37" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="17" t="s">
+      <c r="A38" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H38" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="I38" s="17">
-        <v>5</v>
-      </c>
-      <c r="J38" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="K38">
-        <v>5</v>
-      </c>
-      <c r="L38" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="M38">
-        <v>2</v>
-      </c>
-      <c r="N38" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="O38">
-        <v>2</v>
+      <c r="H38" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" s="29">
+        <v>24</v>
       </c>
       <c r="U38" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
-        <v>69</v>
+      <c r="A39" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>57</v>
@@ -2452,7 +2493,7 @@
         <v>81</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F39" s="28" t="s">
         <v>8</v>
@@ -2478,7 +2519,7 @@
         <v>81</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>8</v>
@@ -2504,7 +2545,7 @@
         <v>81</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F41" s="28" t="s">
         <v>8</v>
@@ -2521,7 +2562,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>57</v>
@@ -2530,7 +2571,7 @@
         <v>81</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="F42" s="28" t="s">
         <v>8</v>
@@ -2547,7 +2588,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>57</v>
@@ -2556,7 +2597,7 @@
         <v>81</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F43" s="28" t="s">
         <v>8</v>
@@ -2565,7 +2606,7 @@
         <v>83</v>
       </c>
       <c r="I43" s="29">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="U43" s="34">
         <v>1</v>
@@ -2585,7 +2626,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="H44" s="31" t="s">
         <v>83</v>
@@ -2611,7 +2652,7 @@
         <v>11</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H45" s="31" t="s">
         <v>83</v>
@@ -2624,8 +2665,8 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
-        <v>26</v>
+      <c r="A46" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>57</v>
@@ -2637,7 +2678,7 @@
         <v>11</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H46" s="31" t="s">
         <v>83</v>
@@ -2650,8 +2691,8 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
-        <v>69</v>
+      <c r="A47" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="C47" s="26" t="s">
         <v>57</v>
@@ -2663,13 +2704,13 @@
         <v>11</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H47" s="31" t="s">
         <v>83</v>
       </c>
       <c r="I47" s="29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U47" s="34">
         <v>1</v>
@@ -2689,7 +2730,7 @@
         <v>11</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H48" s="31" t="s">
         <v>83</v>
@@ -2703,7 +2744,7 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>57</v>
@@ -2715,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H49" s="31" t="s">
         <v>83</v>
@@ -2741,7 +2782,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="H50" s="31" t="s">
         <v>83</v>
@@ -2767,7 +2808,7 @@
         <v>11</v>
       </c>
       <c r="F51" s="28" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="H51" s="31" t="s">
         <v>83</v>
@@ -2781,7 +2822,7 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>57</v>
@@ -2793,7 +2834,7 @@
         <v>11</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="H52" s="31" t="s">
         <v>83</v>
@@ -2807,7 +2848,7 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="C53" s="26" t="s">
         <v>57</v>
@@ -2819,7 +2860,7 @@
         <v>11</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="H53" s="31" t="s">
         <v>83</v>
@@ -2832,8 +2873,8 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
-        <v>26</v>
+      <c r="A54" s="32" t="s">
+        <v>82</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>57</v>
@@ -2845,21 +2886,21 @@
         <v>11</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H54" s="31" t="s">
         <v>83</v>
       </c>
       <c r="I54" s="29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U54" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
-        <v>82</v>
+      <c r="A55" s="30" t="s">
+        <v>78</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>57</v>
@@ -2871,13 +2912,13 @@
         <v>11</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="H55" s="31" t="s">
         <v>83</v>
       </c>
       <c r="I55" s="29">
-        <v>2</v>
+        <v>504</v>
       </c>
       <c r="U55" s="34">
         <v>1</v>
@@ -2903,7 +2944,7 @@
         <v>83</v>
       </c>
       <c r="I56" s="29">
-        <v>504</v>
+        <v>2032</v>
       </c>
       <c r="U56" s="34">
         <v>1</v>
@@ -2920,7 +2961,7 @@
         <v>81</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="F57" s="28" t="s">
         <v>32</v>
@@ -2929,7 +2970,7 @@
         <v>83</v>
       </c>
       <c r="I57" s="29">
-        <v>2032</v>
+        <v>1008</v>
       </c>
       <c r="U57" s="34">
         <v>1</v>
@@ -2946,16 +2987,16 @@
         <v>81</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="H58" s="31" t="s">
         <v>83</v>
       </c>
       <c r="I58" s="29">
-        <v>1008</v>
+        <v>504</v>
       </c>
       <c r="U58" s="34">
         <v>1</v>
@@ -2981,7 +3022,7 @@
         <v>83</v>
       </c>
       <c r="I59" s="29">
-        <v>504</v>
+        <v>2032</v>
       </c>
       <c r="U59" s="34">
         <v>1</v>
@@ -2998,7 +3039,7 @@
         <v>81</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="F60" s="28" t="s">
         <v>63</v>
@@ -3007,76 +3048,76 @@
         <v>83</v>
       </c>
       <c r="I60" s="29">
-        <v>2032</v>
+        <v>1008</v>
       </c>
       <c r="U60" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F61" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="H61" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="I61" s="29">
-        <v>1008</v>
-      </c>
-      <c r="U61" s="34">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="I62" s="7">
+        <v>6</v>
+      </c>
+      <c r="U62" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" s="5" t="s">
+      <c r="A63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F63" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H63" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="I63" s="7">
-        <v>6</v>
-      </c>
-      <c r="U63" s="1">
+      <c r="H63" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="I63" s="33">
+        <v>3</v>
+      </c>
+      <c r="K63" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="34" t="s">
         <v>99</v>
       </c>
       <c r="E64" s="33" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="F64" s="33" t="s">
         <v>8</v>
@@ -3085,35 +3126,9 @@
         <v>101</v>
       </c>
       <c r="I64" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K64" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E65" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="F65" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H65" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="I65" s="33">
-        <v>4</v>
-      </c>
-      <c r="K65" s="33">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
6-add logging label for quick searching
</commit_message>
<xml_diff>
--- a/Resources/6-data.xlsx
+++ b/Resources/6-data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
@@ -11,12 +11,12 @@
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="133">
   <si>
     <t>Order type</t>
   </si>
@@ -409,13 +409,19 @@
   </si>
   <si>
     <t>3014014970</t>
+  </si>
+  <si>
+    <t>3014014971</t>
+  </si>
+  <si>
+    <t>3014014972</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,19 +631,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59996337778862885"/>
+        <fgColor theme="4" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -648,19 +654,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
+        <fgColor theme="5" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59996337778862885"/>
+        <fgColor theme="5" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -671,19 +677,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79995117038483843"/>
+        <fgColor theme="6" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59996337778862885"/>
+        <fgColor theme="6" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -694,19 +700,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
+        <fgColor theme="7" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59996337778862885"/>
+        <fgColor theme="7" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -717,19 +723,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79995117038483843"/>
+        <fgColor theme="8" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
+        <fgColor theme="8" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -740,19 +746,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
+        <fgColor theme="9" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+        <fgColor theme="9" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -785,7 +791,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.49995422223578601"/>
+        <color theme="4" tint="0.49995422223579"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,7 +800,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519242"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,47 +888,47 @@
   <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -932,147 +938,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="47">
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="true"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="true"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="true"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="true"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="true"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="true"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="true"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="true"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="true"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="true"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="true"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="true"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="true"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="true"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="true"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="true"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="true"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="true"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="true"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="true"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="true"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="true"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="true"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="true"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="true"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="true"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="true"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="true"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="true"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="true"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="true"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 11" xfId="46"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="44"/>
     <cellStyle name="Normal 3" xfId="43"/>
     <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="true"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="true"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="true"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="true"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1362,41 +1363,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="34" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="34" customWidth="1"/>
-    <col min="3" max="3" width="15" style="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="34" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="34" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="34" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="34" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="34" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="34" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" style="34" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" style="34" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="34" customWidth="true"/>
+    <col min="2" max="2" width="13.7109375" style="34" customWidth="true"/>
+    <col min="3" max="3" width="15" style="34" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.85546875" style="34" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="13.5703125" style="34" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="16" style="34" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="16" style="34" customWidth="true"/>
+    <col min="8" max="8" width="15.7109375" style="34" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="10.7109375" style="34" customWidth="true"/>
+    <col min="10" max="10" width="12.7109375" style="34" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="10.7109375" style="34" customWidth="true"/>
+    <col min="12" max="12" width="12.7109375" style="34" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="12.7109375" style="34" customWidth="true"/>
+    <col min="14" max="14" width="11.5703125" style="34" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="10.7109375" style="34" customWidth="true"/>
+    <col min="16" max="16" width="10.7109375" style="34" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="10.7109375" style="34" customWidth="true"/>
+    <col min="18" max="18" width="18.42578125" style="34" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="6.85546875" style="34" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="18.28515625" style="34" bestFit="true" customWidth="true"/>
+    <col min="21" max="21" width="13.85546875" style="34" customWidth="true"/>
+    <col min="22" max="22" width="11.85546875" style="34" customWidth="true"/>
     <col min="23" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="34" t="s">
         <v>12</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="32" t="s">
         <v>118</v>
       </c>
@@ -1490,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="V2" s="34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="32" t="s">
         <v>120</v>
       </c>
@@ -1519,10 +1520,10 @@
         <v>1</v>
       </c>
       <c r="V3" s="34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="34" t="s">
         <v>97</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="36" t="s">
         <v>96</v>
       </c>
@@ -1586,42 +1587,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="5.7109375" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="6" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="12.85546875" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="8.42578125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="4.85546875" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="9" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="7.85546875" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="11.42578125" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="6.85546875" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="11" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="10.42578125" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="9.140625" bestFit="true" customWidth="true"/>
+    <col min="15" max="16" width="9.5703125" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="10.85546875" customWidth="true"/>
+    <col min="18" max="18" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="12" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="8.85546875" bestFit="true" customWidth="true"/>
+    <col min="21" max="21" width="11.85546875" bestFit="true" customWidth="true"/>
+    <col min="22" max="22" width="9.85546875" bestFit="true" customWidth="true"/>
+    <col min="23" max="23" width="16" bestFit="true" customWidth="true"/>
+    <col min="24" max="24" width="13.5703125" bestFit="true" customWidth="true"/>
+    <col min="25" max="25" width="9.28515625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1704,39 +1705,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" style="33" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="true"/>
+    <col min="2" max="2" width="13.7109375" customWidth="true"/>
+    <col min="3" max="4" width="14.28515625" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="13.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="16" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="16" customWidth="true"/>
+    <col min="8" max="8" width="15.7109375" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="10.7109375" customWidth="true"/>
+    <col min="10" max="10" width="12.7109375" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="10.7109375" customWidth="true"/>
+    <col min="12" max="12" width="12.7109375" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="12.7109375" customWidth="true"/>
+    <col min="14" max="14" width="11.5703125" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="10.7109375" customWidth="true"/>
+    <col min="16" max="16" width="10.7109375" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="10.7109375" customWidth="true"/>
+    <col min="18" max="18" width="18.42578125" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="6.85546875" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="18.28515625" bestFit="true" customWidth="true"/>
+    <col min="21" max="21" width="13.85546875" customWidth="true"/>
+    <col min="22" max="22" width="14.42578125" style="33" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" s="34" customFormat="true" ht="30">
       <c r="A2" s="33" t="s">
         <v>70</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>3013697282</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="34" customFormat="true">
       <c r="A3" s="33" t="s">
         <v>103</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>3013697283</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="33" t="s">
         <v>70</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>3013697284</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" ht="30">
       <c r="A5" s="33" t="s">
         <v>70</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="33" t="s">
         <v>103</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="33" t="s">
         <v>70</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>3013697287</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" s="34" customFormat="true">
       <c r="A8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
@@ -2026,7 +2027,7 @@
       </c>
       <c r="V8" s="33"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="13" t="s">
         <v>71</v>
       </c>
@@ -2084,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="13" t="s">
         <v>24</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
@@ -2139,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="13" t="s">
         <v>72</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="13" t="s">
         <v>26</v>
       </c>
@@ -2217,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="13" t="s">
         <v>26</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="13" t="s">
         <v>72</v>
       </c>
@@ -2295,7 +2296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="13" t="s">
         <v>26</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="13" t="s">
         <v>26</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="13" t="s">
         <v>74</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="13" t="s">
         <v>74</v>
       </c>
@@ -2477,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="14" t="s">
         <v>75</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="13" t="s">
         <v>76</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="13" t="s">
         <v>77</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" s="13" t="s">
         <v>78</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" s="13" t="s">
         <v>79</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" s="13" t="s">
         <v>78</v>
       </c>
@@ -2633,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" s="14" t="s">
         <v>80</v>
       </c>
@@ -2659,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" s="14" t="s">
         <v>80</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" s="14" t="s">
         <v>80</v>
       </c>
@@ -2711,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="A35" s="13" t="s">
         <v>77</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36">
       <c r="A36" s="15" t="s">
         <v>77</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37">
       <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
@@ -2850,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38">
       <c r="A38" s="32" t="s">
         <v>69</v>
       </c>
@@ -2876,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39">
       <c r="A39" s="30" t="s">
         <v>71</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40">
       <c r="A40" s="30" t="s">
         <v>71</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41">
       <c r="A41" s="30" t="s">
         <v>71</v>
       </c>
@@ -2954,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42">
       <c r="A42" s="30" t="s">
         <v>25</v>
       </c>
@@ -2980,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43">
       <c r="A43" s="30" t="s">
         <v>26</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44">
       <c r="A44" s="30" t="s">
         <v>26</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45">
       <c r="A45" s="30" t="s">
         <v>26</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46">
       <c r="A46" s="32" t="s">
         <v>69</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47">
       <c r="A47" s="30" t="s">
         <v>71</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48">
       <c r="A48" s="30" t="s">
         <v>71</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49">
       <c r="A49" s="30" t="s">
         <v>26</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50">
       <c r="A50" s="30" t="s">
         <v>26</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51">
       <c r="A51" s="30" t="s">
         <v>26</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52">
       <c r="A52" s="30" t="s">
         <v>78</v>
       </c>
@@ -3240,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53">
       <c r="A53" s="30" t="s">
         <v>26</v>
       </c>
@@ -3266,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54">
       <c r="A54" s="32" t="s">
         <v>82</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55">
       <c r="A55" s="30" t="s">
         <v>78</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56">
       <c r="A56" s="30" t="s">
         <v>78</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57">
       <c r="A57" s="30" t="s">
         <v>78</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58">
       <c r="A58" s="30" t="s">
         <v>78</v>
       </c>
@@ -3396,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59">
       <c r="A59" s="30" t="s">
         <v>78</v>
       </c>
@@ -3422,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60">
       <c r="A60" s="30" t="s">
         <v>78</v>
       </c>
@@ -3448,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62">
       <c r="A62" s="13" t="s">
         <v>73</v>
       </c>
@@ -3474,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63">
       <c r="A63" t="s">
         <v>96</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64">
       <c r="A64" t="s">
         <v>97</v>
       </c>

</xml_diff>